<commit_message>
feat: migrate Excel storage to Cloudflare R2
</commit_message>
<xml_diff>
--- a/data/VE3.xlsx
+++ b/data/VE3.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="352">
   <si>
     <t>Liên Hệ</t>
   </si>
@@ -73,7 +73,7 @@
     <t>Ngày xuất</t>
   </si>
   <si>
-    <t>23/12/2025</t>
+    <t>25/12/2025</t>
   </si>
   <si>
     <t>VE3</t>
@@ -2165,7 +2165,7 @@
         <v>1.67518290048E11</v>
       </c>
       <c r="AR12" s="13" t="n">
-        <v>1.65521367792E11</v>
+        <v>1.61151329056E11</v>
       </c>
       <c r="AS12" s="13" t="n">
         <v>1.6977786599E11</v>
@@ -3237,7 +3237,7 @@
         <v>9.631047985E10</v>
       </c>
       <c r="AR20" s="13" t="n">
-        <v>9.5156520517E10</v>
+        <v>9.3271480839E10</v>
       </c>
       <c r="AS20" s="13" t="n">
         <v>1.02288331034E11</v>
@@ -4175,7 +4175,7 @@
         <v>-1.309176843E9</v>
       </c>
       <c r="AR27" s="13" t="n">
-        <v>-1.309176843E9</v>
+        <v>-3.194216521E9</v>
       </c>
       <c r="AS27" s="13" t="n">
         <v>-1.309176843E9</v>
@@ -4443,7 +4443,7 @@
         <v>6.1863710204E10</v>
       </c>
       <c r="AR29" s="13" t="n">
-        <v>5.8884259495E10</v>
+        <v>5.6399260437E10</v>
       </c>
       <c r="AS29" s="13" t="n">
         <v>5.1653447842E10</v>
@@ -4577,7 +4577,7 @@
         <v>6.1933771066E10</v>
       </c>
       <c r="AR30" s="13" t="n">
-        <v>5.8954320357E10</v>
+        <v>5.720902031E10</v>
       </c>
       <c r="AS30" s="13" t="n">
         <v>5.1723508704E10</v>
@@ -4711,7 +4711,7 @@
         <v>-7.0060862E7</v>
       </c>
       <c r="AR31" s="13" t="n">
-        <v>-7.0060862E7</v>
+        <v>-8.09759873E8</v>
       </c>
       <c r="AS31" s="13" t="n">
         <v>-7.0060862E7</v>
@@ -10875,7 +10875,7 @@
         <v>1.77081188131E11</v>
       </c>
       <c r="AR77" s="13" t="n">
-        <v>1.74887210813E11</v>
+        <v>1.70517172077E11</v>
       </c>
       <c r="AS77" s="13" t="n">
         <v>1.78945229828E11</v>
@@ -11009,7 +11009,7 @@
         <v>1.57773124609E11</v>
       </c>
       <c r="AR78" s="13" t="n">
-        <v>1.55533472789E11</v>
+        <v>1.55300891458E11</v>
       </c>
       <c r="AS78" s="13" t="n">
         <v>1.61719884727E11</v>
@@ -11143,7 +11143,7 @@
         <v>1.56200941203E11</v>
       </c>
       <c r="AR79" s="13" t="n">
-        <v>1.53998789383E11</v>
+        <v>1.53766208052E11</v>
       </c>
       <c r="AS79" s="13" t="n">
         <v>1.60632384727E11</v>
@@ -11277,7 +11277,7 @@
         <v>4.553777142E10</v>
       </c>
       <c r="AR80" s="13" t="n">
-        <v>5.0332547894E10</v>
+        <v>4.9922864488E10</v>
       </c>
       <c r="AS80" s="13" t="n">
         <v>5.7564658E10</v>
@@ -11411,7 +11411,7 @@
         <v>3.8192058394E10</v>
       </c>
       <c r="AR81" s="13" t="n">
-        <v>2.8457882211E10</v>
+        <v>2.8867565617E10</v>
       </c>
       <c r="AS81" s="13" t="n">
         <v>1.7373900745E10</v>
@@ -11545,7 +11545,7 @@
         <v>5.84371361E8</v>
       </c>
       <c r="AR82" s="13" t="n">
-        <v>9.94525528E8</v>
+        <v>7.61944197E8</v>
       </c>
       <c r="AS82" s="13" t="n">
         <v>4.40267285E8</v>
@@ -15077,7 +15077,7 @@
         <v>1.9308063522E10</v>
       </c>
       <c r="AR109" s="13" t="n">
-        <v>1.9353738024E10</v>
+        <v>1.5216280619E10</v>
       </c>
       <c r="AS109" s="13" t="n">
         <v>1.7225345101E10</v>
@@ -15211,7 +15211,7 @@
         <v>1.9308063522E10</v>
       </c>
       <c r="AR110" s="13" t="n">
-        <v>1.9353738024E10</v>
+        <v>1.5216280619E10</v>
       </c>
       <c r="AS110" s="13" t="n">
         <v>1.7225345101E10</v>
@@ -15479,7 +15479,7 @@
         <v>0.0</v>
       </c>
       <c r="AR112" s="13" t="n">
-        <v>0.0</v>
+        <v>1.31971E10</v>
       </c>
       <c r="AS112" s="13" t="n">
         <v>0.0</v>
@@ -17087,7 +17087,7 @@
         <v>3.557594812E9</v>
       </c>
       <c r="AR124" s="13" t="n">
-        <v>3.603269314E9</v>
+        <v>-5.34188091E8</v>
       </c>
       <c r="AS124" s="13" t="n">
         <v>1.474876391E9</v>
@@ -17355,7 +17355,7 @@
         <v>3.1010639E7</v>
       </c>
       <c r="AR126" s="13" t="n">
-        <v>1.02136629E8</v>
+        <v>-4.035320776E9</v>
       </c>
       <c r="AS126" s="13" t="n">
         <v>-2.026256294E9</v>
@@ -18293,7 +18293,7 @@
         <v>1.77081188131E11</v>
       </c>
       <c r="AR133" s="13" t="n">
-        <v>1.74887210813E11</v>
+        <v>1.70517172077E11</v>
       </c>
       <c r="AS133" s="13" t="n">
         <v>1.78945229828E11</v>
@@ -19113,7 +19113,7 @@
         <v>-1.0125237753E10</v>
       </c>
       <c r="AR15" s="17" t="n">
-        <v>-4.2960150849E10</v>
+        <v>-4.369984986E10</v>
       </c>
       <c r="AS15" s="17" t="n">
         <v>-5.1933891605E10</v>
@@ -19247,7 +19247,7 @@
         <v>3.21071965E8</v>
       </c>
       <c r="AR16" s="17" t="n">
-        <v>3.177567078E9</v>
+        <v>2.437868067E9</v>
       </c>
       <c r="AS16" s="17" t="n">
         <v>2.463336225E9</v>
@@ -19515,7 +19515,7 @@
         <v>-2.10680367E8</v>
       </c>
       <c r="AR18" s="17" t="n">
-        <v>-1.453294884E9</v>
+        <v>-2.503109684E9</v>
       </c>
       <c r="AS18" s="17" t="n">
         <v>-2.46416167E9</v>
@@ -19649,7 +19649,7 @@
         <v>-2.10680367E8</v>
       </c>
       <c r="AR19" s="17" t="n">
-        <v>-1.453294884E9</v>
+        <v>-2.492270425E9</v>
       </c>
       <c r="AS19" s="17" t="n">
         <v>-2.46416167E9</v>
@@ -20051,7 +20051,7 @@
         <v>-1.21767968E8</v>
       </c>
       <c r="AR22" s="17" t="n">
-        <v>-1.534551901E9</v>
+        <v>-4.115076826E9</v>
       </c>
       <c r="AS22" s="17" t="n">
         <v>-2.166092144E9</v>
@@ -20185,7 +20185,7 @@
         <v>5.0210267E7</v>
       </c>
       <c r="AR23" s="17" t="n">
-        <v>3.41347624E8</v>
+        <v>-4.028691112E9</v>
       </c>
       <c r="AS23" s="17" t="n">
         <v>-2.117784986E9</v>
@@ -20855,7 +20855,7 @@
         <v>3.8763299E7</v>
       </c>
       <c r="AR28" s="17" t="n">
-        <v>2.95954661E8</v>
+        <v>-4.074084075E9</v>
       </c>
       <c r="AS28" s="17" t="n">
         <v>-2.128392923E9</v>
@@ -20989,7 +20989,7 @@
         <v>-7752660.0</v>
       </c>
       <c r="AR29" s="17" t="n">
-        <v>-2.24828671E8</v>
+        <v>7752660.0</v>
       </c>
       <c r="AS29" s="17" t="n">
         <v>0.0</v>
@@ -21123,7 +21123,7 @@
         <v>-7752660.0</v>
       </c>
       <c r="AR30" s="17" t="n">
-        <v>-2.24828671E8</v>
+        <v>7752660.0</v>
       </c>
       <c r="AS30" s="17" t="n">
         <v>0.0</v>
@@ -21391,7 +21391,7 @@
         <v>3.1010639E7</v>
       </c>
       <c r="AR32" s="17" t="n">
-        <v>7.112599E7</v>
+        <v>-4.066331415E9</v>
       </c>
       <c r="AS32" s="17" t="n">
         <v>-2.128392923E9</v>
@@ -21659,7 +21659,7 @@
         <v>3.1010639E7</v>
       </c>
       <c r="AR34" s="17" t="n">
-        <v>7.112599E7</v>
+        <v>-4.066331415E9</v>
       </c>
       <c r="AS34" s="17" t="n">
         <v>-2.128392923E9</v>
@@ -21793,7 +21793,7 @@
         <v>23.0</v>
       </c>
       <c r="AR35" s="17" t="n">
-        <v>54.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS35" s="17" t="n">
         <v>-1613.0</v>
@@ -21927,7 +21927,7 @@
         <v>23.0</v>
       </c>
       <c r="AR36" s="17" t="n">
-        <v>54.0</v>
+        <v>0.0</v>
       </c>
       <c r="AS36" s="17" t="n">
         <v>-1613.0</v>
@@ -21985,7 +21985,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF32B87-0276-EF4E-963C-ED48B34C3BF9}">
-  <dimension ref="A1:AQ60"/>
+  <dimension ref="A1:AR60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -22036,6 +22036,7 @@
     <col min="41" max="41" width="16.28515625" customWidth="true" bestFit="true"/>
     <col min="42" max="42" width="16.28515625" customWidth="true" bestFit="true"/>
     <col min="43" max="43" width="16.28515625" customWidth="true" bestFit="true"/>
+    <col min="44" max="44" width="16.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -22206,6 +22207,9 @@
         <v>48</v>
       </c>
       <c r="AQ11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR11" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -22336,6 +22340,9 @@
       <c r="AQ12" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR12" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
@@ -22464,6 +22471,9 @@
       <c r="AQ13" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR13" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="24" t="s">
@@ -22592,6 +22602,9 @@
       <c r="AQ14" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR14" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="24" t="s">
@@ -22720,6 +22733,9 @@
       <c r="AQ15" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR15" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="24" t="s">
@@ -22848,6 +22864,9 @@
       <c r="AQ16" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR16" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="24" t="s">
@@ -22976,6 +22995,9 @@
       <c r="AQ17" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR17" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="24" t="s">
@@ -23104,6 +23126,9 @@
       <c r="AQ18" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR18" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="s">
@@ -23232,6 +23257,9 @@
       <c r="AQ19" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR19" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="24" t="s">
@@ -23360,6 +23388,9 @@
       <c r="AQ20" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR20" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="24" t="s">
@@ -23488,6 +23519,9 @@
       <c r="AQ21" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR21" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="24" t="s">
@@ -23614,6 +23648,9 @@
         <v>-2.3322930349E10</v>
       </c>
       <c r="AQ22" s="21" t="n">
+        <v>1.535737517E9</v>
+      </c>
+      <c r="AR22" s="21" t="n">
         <v>-5.564069578E9</v>
       </c>
     </row>
@@ -23744,6 +23781,9 @@
       <c r="AQ23" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR23" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="22" t="s">
@@ -23872,6 +23912,9 @@
       <c r="AQ24" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR24" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="22" t="s">
@@ -24000,6 +24043,9 @@
       <c r="AQ25" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR25" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="22" t="s">
@@ -24128,6 +24174,9 @@
       <c r="AQ26" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR26" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="22" t="s">
@@ -24256,6 +24305,9 @@
       <c r="AQ27" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR27" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="22" t="s">
@@ -24384,6 +24436,9 @@
       <c r="AQ28" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR28" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="22" t="s">
@@ -24512,6 +24567,9 @@
       <c r="AQ29" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR29" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="22" t="s">
@@ -24640,6 +24698,9 @@
       <c r="AQ30" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR30" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="22" t="s">
@@ -24768,6 +24829,9 @@
       <c r="AQ31" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR31" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="22" t="s">
@@ -24896,6 +24960,9 @@
       <c r="AQ32" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR32" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="24" t="s">
@@ -25022,6 +25089,9 @@
         <v>4.1053592E7</v>
       </c>
       <c r="AQ33" s="21" t="n">
+        <v>4.115511E7</v>
+      </c>
+      <c r="AR33" s="21" t="n">
         <v>4.8825357E7</v>
       </c>
     </row>
@@ -25152,6 +25222,9 @@
       <c r="AQ34" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR34" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="22" t="s">
@@ -25280,6 +25353,9 @@
       <c r="AQ35" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR35" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="22" t="s">
@@ -25408,6 +25484,9 @@
       <c r="AQ36" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR36" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="22" t="s">
@@ -25536,6 +25615,9 @@
       <c r="AQ37" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR37" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="22" t="s">
@@ -25664,6 +25746,9 @@
       <c r="AQ38" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR38" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="22" t="s">
@@ -25792,6 +25877,9 @@
       <c r="AQ39" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR39" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="22" t="s">
@@ -25918,6 +26006,9 @@
         <v>4.1053592E7</v>
       </c>
       <c r="AQ40" s="21" t="n">
+        <v>4.115511E7</v>
+      </c>
+      <c r="AR40" s="21" t="n">
         <v>4.8825357E7</v>
       </c>
     </row>
@@ -26046,6 +26137,9 @@
         <v>5.186838912E9</v>
       </c>
       <c r="AQ41" s="21" t="n">
+        <v>1.353137391E9</v>
+      </c>
+      <c r="AR41" s="21" t="n">
         <v>4.447118341E9</v>
       </c>
     </row>
@@ -26176,6 +26270,9 @@
       <c r="AQ42" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR42" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="22" t="s">
@@ -26304,6 +26401,9 @@
       <c r="AQ43" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR43" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="22" t="s">
@@ -26430,6 +26530,9 @@
         <v>2.5736178591E10</v>
       </c>
       <c r="AQ44" s="21" t="n">
+        <v>1.9026216924E10</v>
+      </c>
+      <c r="AR44" s="21" t="n">
         <v>3.2822743201E10</v>
       </c>
     </row>
@@ -26558,6 +26661,9 @@
         <v>-2.0549339679E10</v>
       </c>
       <c r="AQ45" s="21" t="n">
+        <v>-1.7673079533E10</v>
+      </c>
+      <c r="AR45" s="21" t="n">
         <v>-2.837562486E10</v>
       </c>
     </row>
@@ -26688,6 +26794,9 @@
       <c r="AQ46" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR46" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="22" t="s">
@@ -26816,6 +26925,9 @@
       <c r="AQ47" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR47" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="22" t="s">
@@ -26944,6 +27056,9 @@
       <c r="AQ48" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR48" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="24" t="s">
@@ -27070,6 +27185,9 @@
         <v>-1.8095037845E10</v>
       </c>
       <c r="AQ49" s="21" t="n">
+        <v>2.930030018E9</v>
+      </c>
+      <c r="AR49" s="21" t="n">
         <v>-1.06812588E9</v>
       </c>
     </row>
@@ -27198,6 +27316,9 @@
         <v>2.3883493806E10</v>
       </c>
       <c r="AQ50" s="21" t="n">
+        <v>5.788455961E9</v>
+      </c>
+      <c r="AR50" s="21" t="n">
         <v>8.718485979E9</v>
       </c>
     </row>
@@ -27328,6 +27449,9 @@
       <c r="AQ51" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR51" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="24" t="s">
@@ -27454,6 +27578,9 @@
         <v>5.788455961E9</v>
       </c>
       <c r="AQ52" s="21" t="n">
+        <v>8.718485979E9</v>
+      </c>
+      <c r="AR52" s="21" t="n">
         <v>7.650360099E9</v>
       </c>
     </row>
@@ -27495,7 +27622,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B10:I10"/>
-    <mergeCell ref="K10:AQ10"/>
+    <mergeCell ref="K10:AR10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A58" r:id="rId1" display="https://www.vietcap.com.vn/" xr:uid="{2404128C-51EF-8E44-9BE0-4A8D207DD5D8}"/>
@@ -27509,7 +27636,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACDB1F9-64B2-F64B-91A6-B0AAFF7D49C4}">
-  <dimension ref="A1:AL176"/>
+  <dimension ref="A1:AM176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -27555,6 +27682,7 @@
     <col min="36" max="36" width="15.625" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="15.625" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="15.625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="15.625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27710,6 +27838,9 @@
         <v>48</v>
       </c>
       <c r="AL11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM11" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -27823,6 +27954,9 @@
         <v>5.788455961E9</v>
       </c>
       <c r="AL12" s="25" t="n">
+        <v>8.718485979E9</v>
+      </c>
+      <c r="AM12" s="25" t="n">
         <v>1.4405360099E10</v>
       </c>
     </row>
@@ -27936,6 +28070,9 @@
         <v>1.9073931E7</v>
       </c>
       <c r="AL13" s="25" t="n">
+        <v>9583278.0</v>
+      </c>
+      <c r="AM13" s="25" t="n">
         <v>5965112.0</v>
       </c>
     </row>
@@ -28049,6 +28186,9 @@
         <v>2.9271982E8</v>
       </c>
       <c r="AL14" s="25" t="n">
+        <v>2.253902701E9</v>
+      </c>
+      <c r="AM14" s="25" t="n">
         <v>7.622732777E9</v>
       </c>
     </row>
@@ -28162,6 +28302,9 @@
         <v>2.166221E7</v>
       </c>
       <c r="AL15" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AM15" s="25" t="n">
         <v>2.166221E7</v>
       </c>
     </row>
@@ -28275,6 +28418,9 @@
         <v>5.455E9</v>
       </c>
       <c r="AL16" s="25" t="n">
+        <v>6.455E9</v>
+      </c>
+      <c r="AM16" s="25" t="n">
         <v>6.755E9</v>
       </c>
     </row>
@@ -28390,6 +28536,9 @@
       <c r="AL17" s="25" t="n">
         <v>1.2E9</v>
       </c>
+      <c r="AM17" s="25" t="n">
+        <v>1.2E9</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
@@ -28503,6 +28652,9 @@
       <c r="AL18" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM18" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="26" t="s">
@@ -28616,6 +28768,9 @@
       <c r="AL19" s="25" t="n">
         <v>1.2E9</v>
       </c>
+      <c r="AM19" s="25" t="n">
+        <v>1.2E9</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
@@ -28729,6 +28884,9 @@
       <c r="AL20" s="25" t="n">
         <v>1.2E9</v>
       </c>
+      <c r="AM20" s="25" t="n">
+        <v>1.2E9</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="26" t="s">
@@ -28842,6 +29000,9 @@
       <c r="AL21" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM21" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="26" t="s">
@@ -28955,6 +29116,9 @@
       <c r="AL22" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM22" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="26" t="s">
@@ -29068,6 +29232,9 @@
       <c r="AL23" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM23" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
@@ -29179,6 +29346,9 @@
         <v>0.0</v>
       </c>
       <c r="AL24" s="25" t="n">
+        <v>2.0066915597E10</v>
+      </c>
+      <c r="AM24" s="25" t="n">
         <v>1.8020263297E10</v>
       </c>
     </row>
@@ -29294,6 +29464,9 @@
       <c r="AL25" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM25" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="26" t="s">
@@ -29407,6 +29580,9 @@
       <c r="AL26" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM26" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
@@ -29520,6 +29696,9 @@
       <c r="AL27" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM27" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
@@ -29631,6 +29810,9 @@
         <v>0.0</v>
       </c>
       <c r="AL28" s="25" t="n">
+        <v>2.0066915597E10</v>
+      </c>
+      <c r="AM28" s="25" t="n">
         <v>1.8020263297E10</v>
       </c>
     </row>
@@ -29744,6 +29926,9 @@
         <v>6.1933771066E10</v>
       </c>
       <c r="AL29" s="25" t="n">
+        <v>5.720902031E10</v>
+      </c>
+      <c r="AM29" s="25" t="n">
         <v>5.1723508704E10</v>
       </c>
     </row>
@@ -29859,6 +30044,9 @@
       <c r="AL30" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM30" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="26" t="s">
@@ -29970,6 +30158,9 @@
         <v>9.690260364E9</v>
       </c>
       <c r="AL31" s="25" t="n">
+        <v>4.103165179E9</v>
+      </c>
+      <c r="AM31" s="25" t="n">
         <v>3.250679543E9</v>
       </c>
     </row>
@@ -30083,6 +30274,9 @@
         <v>5.173346E7</v>
       </c>
       <c r="AL32" s="25" t="n">
+        <v>3.878596E7</v>
+      </c>
+      <c r="AM32" s="25" t="n">
         <v>2.137396E7</v>
       </c>
     </row>
@@ -30196,6 +30390,9 @@
         <v>5.0110651514E10</v>
       </c>
       <c r="AL33" s="25" t="n">
+        <v>5.0882321211E10</v>
+      </c>
+      <c r="AM33" s="25" t="n">
         <v>4.6502305974E10</v>
       </c>
     </row>
@@ -30309,6 +30506,9 @@
         <v>2.081125728E9</v>
       </c>
       <c r="AL34" s="25" t="n">
+        <v>2.18474796E9</v>
+      </c>
+      <c r="AM34" s="25" t="n">
         <v>1.949149227E9</v>
       </c>
     </row>
@@ -30424,6 +30624,9 @@
       <c r="AL35" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM35" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="26" t="s">
@@ -30537,6 +30740,9 @@
       <c r="AL36" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM36" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="26" t="s">
@@ -30650,6 +30856,9 @@
       <c r="AL37" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM37" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="26" t="s">
@@ -30763,6 +30972,9 @@
       <c r="AL38" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM38" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="28" t="s">
@@ -30876,6 +31088,9 @@
       <c r="AL39" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM39" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="26" t="s">
@@ -30989,6 +31204,9 @@
       <c r="AL40" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM40" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="26" t="s">
@@ -31102,6 +31320,9 @@
       <c r="AL41" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM41" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="26" t="s">
@@ -31215,6 +31436,9 @@
       <c r="AL42" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM42" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="26" t="s">
@@ -31328,6 +31552,9 @@
       <c r="AL43" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM43" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="28" t="s">
@@ -31441,6 +31668,9 @@
       <c r="AL44" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM44" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="26" t="s">
@@ -31554,6 +31784,9 @@
       <c r="AL45" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM45" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="26" t="s">
@@ -31667,6 +31900,9 @@
       <c r="AL46" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM46" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="26" t="s">
@@ -31780,6 +32016,9 @@
       <c r="AL47" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM47" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="26" t="s">
@@ -31893,6 +32132,9 @@
       <c r="AL48" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM48" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="28" t="s">
@@ -32006,6 +32248,9 @@
       <c r="AL49" s="25" t="n">
         <v>1.7854444979E10</v>
       </c>
+      <c r="AM49" s="25" t="n">
+        <v>1.7854444979E10</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="26" t="s">
@@ -32119,6 +32364,9 @@
       <c r="AL50" s="25" t="n">
         <v>1.7854444979E10</v>
       </c>
+      <c r="AM50" s="25" t="n">
+        <v>1.7854444979E10</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="26" t="s">
@@ -32232,6 +32480,9 @@
       <c r="AL51" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM51" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="26" t="s">
@@ -32345,6 +32596,9 @@
       <c r="AL52" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM52" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="28" t="s">
@@ -32456,6 +32710,9 @@
         <v>0.0</v>
       </c>
       <c r="AL53" s="25" t="n">
+        <v>1.2251956933E10</v>
+      </c>
+      <c r="AM53" s="25" t="n">
         <v>1.2430129078E10</v>
       </c>
     </row>
@@ -32571,6 +32828,9 @@
       <c r="AL54" s="25" t="n">
         <v>1.189633332E10</v>
       </c>
+      <c r="AM54" s="25" t="n">
+        <v>1.189633332E10</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="26" t="s">
@@ -32682,6 +32942,9 @@
         <v>0.0</v>
       </c>
       <c r="AL55" s="25" t="n">
+        <v>3.55623613E8</v>
+      </c>
+      <c r="AM55" s="25" t="n">
         <v>5.33795758E8</v>
       </c>
     </row>
@@ -32797,6 +33060,9 @@
       <c r="AL56" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM56" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="28" t="s">
@@ -32910,6 +33176,9 @@
       <c r="AL57" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM57" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="26" t="s">
@@ -33023,6 +33292,9 @@
       <c r="AL58" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM58" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="26" t="s">
@@ -33136,6 +33408,9 @@
       <c r="AL59" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM59" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="26" t="s">
@@ -33249,6 +33524,9 @@
       <c r="AL60" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM60" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="28" t="s">
@@ -33362,6 +33640,9 @@
       <c r="AL61" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM61" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="26" t="s">
@@ -33475,6 +33756,9 @@
       <c r="AL62" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM62" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="26" t="s">
@@ -33588,6 +33872,9 @@
       <c r="AL63" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM63" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="26" t="s">
@@ -33701,6 +33988,9 @@
       <c r="AL64" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM64" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="28" t="s">
@@ -33814,6 +34104,9 @@
       <c r="AL65" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM65" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="26" t="s">
@@ -33927,6 +34220,9 @@
       <c r="AL66" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM66" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="26" t="s">
@@ -34040,6 +34336,9 @@
       <c r="AL67" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM67" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="26" t="s">
@@ -34153,6 +34452,9 @@
       <c r="AL68" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM68" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="28" t="s">
@@ -34266,6 +34568,9 @@
       <c r="AL69" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM69" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="26" t="s">
@@ -34379,6 +34684,9 @@
       <c r="AL70" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM70" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="26" t="s">
@@ -34492,6 +34800,9 @@
       <c r="AL71" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM71" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="26" t="s">
@@ -34605,6 +34916,9 @@
       <c r="AL72" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM72" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="28" t="s">
@@ -34718,6 +35032,9 @@
       <c r="AL73" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM73" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="26" t="s">
@@ -34831,6 +35148,9 @@
       <c r="AL74" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM74" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="26" t="s">
@@ -34944,6 +35264,9 @@
       <c r="AL75" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM75" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="26" t="s">
@@ -35057,6 +35380,9 @@
       <c r="AL76" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM76" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="26" t="s">
@@ -35170,6 +35496,9 @@
       <c r="AL77" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM77" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="26" t="s">
@@ -35283,6 +35612,9 @@
       <c r="AL78" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM78" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="28" t="s">
@@ -35396,6 +35728,9 @@
       <c r="AL79" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM79" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="26" t="s">
@@ -35509,6 +35844,9 @@
       <c r="AL80" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM80" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="26" t="s">
@@ -35622,6 +35960,9 @@
       <c r="AL81" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM81" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="28" t="s">
@@ -35735,6 +36076,9 @@
       <c r="AL82" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM82" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="26" t="s">
@@ -35848,6 +36192,9 @@
       <c r="AL83" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM83" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="26" t="s">
@@ -35961,6 +36308,9 @@
       <c r="AL84" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM84" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="26" t="s">
@@ -36074,6 +36424,9 @@
       <c r="AL85" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM85" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="28" t="s">
@@ -36187,6 +36540,9 @@
       <c r="AL86" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM86" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="26" t="s">
@@ -36300,6 +36656,9 @@
       <c r="AL87" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM87" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="26" t="s">
@@ -36413,6 +36772,9 @@
       <c r="AL88" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM88" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="26" t="s">
@@ -36526,6 +36888,9 @@
       <c r="AL89" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM89" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="28" t="s">
@@ -36637,6 +37002,9 @@
         <v>5.84371361E8</v>
       </c>
       <c r="AL90" s="25" t="n">
+        <v>7.61944197E8</v>
+      </c>
+      <c r="AM90" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -36752,6 +37120,9 @@
       <c r="AL91" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM91" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="26" t="s">
@@ -36865,6 +37236,9 @@
       <c r="AL92" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM92" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="26" t="s">
@@ -36978,6 +37352,9 @@
       <c r="AL93" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM93" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="26" t="s">
@@ -37089,6 +37466,9 @@
         <v>5.76936293E8</v>
       </c>
       <c r="AL94" s="25" t="n">
+        <v>5.69183633E8</v>
+      </c>
+      <c r="AM94" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -37202,6 +37582,9 @@
         <v>7435068.0</v>
       </c>
       <c r="AL95" s="25" t="n">
+        <v>1.2600818E7</v>
+      </c>
+      <c r="AM95" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -37317,6 +37700,9 @@
       <c r="AL96" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM96" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="26" t="s">
@@ -37428,6 +37814,9 @@
         <v>0.0</v>
       </c>
       <c r="AL97" s="25" t="n">
+        <v>1.80159746E8</v>
+      </c>
+      <c r="AM97" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -37543,6 +37932,9 @@
       <c r="AL98" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM98" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="26" t="s">
@@ -37656,6 +38048,9 @@
       <c r="AL99" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM99" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="28" t="s">
@@ -37769,6 +38164,9 @@
       <c r="AL100" s="25" t="n">
         <v>3.927156375E9</v>
       </c>
+      <c r="AM100" s="25" t="n">
+        <v>3.927156375E9</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="26" t="s">
@@ -37882,6 +38280,9 @@
       <c r="AL101" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM101" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="26" t="s">
@@ -37995,6 +38396,9 @@
       <c r="AL102" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM102" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="26" t="s">
@@ -38108,6 +38512,9 @@
       <c r="AL103" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM103" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="26" t="s">
@@ -38221,6 +38628,9 @@
       <c r="AL104" s="25" t="n">
         <v>3.927156375E9</v>
       </c>
+      <c r="AM104" s="25" t="n">
+        <v>3.927156375E9</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="28" t="s">
@@ -38332,6 +38742,9 @@
         <v>0.0</v>
       </c>
       <c r="AL105" s="25" t="n">
+        <v>2.331729274E9</v>
+      </c>
+      <c r="AM105" s="25" t="n">
         <v>8.153349836E9</v>
       </c>
     </row>
@@ -38447,6 +38860,9 @@
       <c r="AL106" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM106" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="26" t="s">
@@ -38558,6 +38974,9 @@
         <v>0.0</v>
       </c>
       <c r="AL107" s="25" t="n">
+        <v>1.3122478E8</v>
+      </c>
+      <c r="AM107" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -38671,6 +39090,9 @@
         <v>0.0</v>
       </c>
       <c r="AL108" s="25" t="n">
+        <v>2.70051751E8</v>
+      </c>
+      <c r="AM108" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -38784,6 +39206,9 @@
         <v>0.0</v>
       </c>
       <c r="AL109" s="25" t="n">
+        <v>4.9571326E7</v>
+      </c>
+      <c r="AM109" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -38897,6 +39322,9 @@
         <v>0.0</v>
       </c>
       <c r="AL110" s="25" t="n">
+        <v>5.3049691E7</v>
+      </c>
+      <c r="AM110" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -39012,6 +39440,9 @@
       <c r="AL111" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM111" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="26" t="s">
@@ -39125,6 +39556,9 @@
       <c r="AL112" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM112" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="26" t="s">
@@ -39238,6 +39672,9 @@
       <c r="AL113" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM113" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="26" t="s">
@@ -39349,6 +39786,9 @@
         <v>0.0</v>
       </c>
       <c r="AL114" s="25" t="n">
+        <v>1.827831726E9</v>
+      </c>
+      <c r="AM114" s="25" t="n">
         <v>8.153349836E9</v>
       </c>
     </row>
@@ -39464,6 +39904,9 @@
       <c r="AL115" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM115" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="26" t="s">
@@ -39577,6 +40020,9 @@
       <c r="AL116" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM116" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="26" t="s">
@@ -39690,6 +40136,9 @@
       <c r="AL117" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM117" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="26" t="s">
@@ -39803,6 +40252,9 @@
       <c r="AL118" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM118" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="26" t="s">
@@ -39916,6 +40368,9 @@
       <c r="AL119" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM119" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="26" t="s">
@@ -40029,6 +40484,9 @@
       <c r="AL120" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM120" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="28" t="s">
@@ -40142,6 +40600,9 @@
       <c r="AL121" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM121" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="26" t="s">
@@ -40255,6 +40716,9 @@
       <c r="AL122" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM122" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="26" t="s">
@@ -40368,6 +40832,9 @@
       <c r="AL123" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM123" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="28" t="s">
@@ -40479,6 +40946,9 @@
         <v>1.0446309718E10</v>
       </c>
       <c r="AL124" s="25" t="n">
+        <v>4.6137717927E10</v>
+      </c>
+      <c r="AM124" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -40592,6 +41062,9 @@
         <v>0.0</v>
       </c>
       <c r="AL125" s="25" t="n">
+        <v>4.6137717927E10</v>
+      </c>
+      <c r="AM125" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -40707,6 +41180,9 @@
       <c r="AL126" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM126" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="26" t="s">
@@ -40820,6 +41296,9 @@
       <c r="AL127" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM127" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="28" t="s">
@@ -40933,6 +41412,9 @@
       <c r="AL128" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM128" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="26" t="s">
@@ -41046,6 +41528,9 @@
       <c r="AL129" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM129" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="26" t="s">
@@ -41159,6 +41644,9 @@
       <c r="AL130" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM130" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="26" t="s">
@@ -41272,6 +41760,9 @@
       <c r="AL131" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM131" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="26" t="s">
@@ -41385,6 +41876,9 @@
       <c r="AL132" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM132" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="26" t="s">
@@ -41498,6 +41992,9 @@
       <c r="AL133" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM133" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="26" t="s">
@@ -41611,6 +42108,9 @@
       <c r="AL134" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM134" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="28" t="s">
@@ -41722,6 +42222,9 @@
         <v>1.0125237753E10</v>
       </c>
       <c r="AL135" s="25" t="n">
+        <v>4.369984986E10</v>
+      </c>
+      <c r="AM135" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -41835,6 +42338,9 @@
         <v>0.0</v>
       </c>
       <c r="AL136" s="25" t="n">
+        <v>1.0286525301E10</v>
+      </c>
+      <c r="AM136" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -41950,6 +42456,9 @@
       <c r="AL137" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM137" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="26" t="s">
@@ -42061,6 +42570,9 @@
         <v>1.0125237753E10</v>
       </c>
       <c r="AL138" s="25" t="n">
+        <v>3.2673625548E10</v>
+      </c>
+      <c r="AM138" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -42176,6 +42688,9 @@
       <c r="AL139" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM139" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="26" t="s">
@@ -42289,6 +42804,9 @@
       <c r="AL140" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM140" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="26" t="s">
@@ -42402,6 +42920,9 @@
       <c r="AL141" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM141" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="26" t="s">
@@ -42515,6 +43036,9 @@
       <c r="AL142" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM142" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="26" t="s">
@@ -42626,6 +43150,9 @@
         <v>0.0</v>
       </c>
       <c r="AL143" s="25" t="n">
+        <v>7.39699011E8</v>
+      </c>
+      <c r="AM143" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -42739,6 +43266,9 @@
         <v>6.1586637E7</v>
       </c>
       <c r="AL144" s="25" t="n">
+        <v>1.51627331E8</v>
+      </c>
+      <c r="AM144" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -42852,6 +43382,9 @@
         <v>6.1586637E7</v>
       </c>
       <c r="AL145" s="25" t="n">
+        <v>2.0622065E7</v>
+      </c>
+      <c r="AM145" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -42967,6 +43500,9 @@
       <c r="AL146" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM146" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="26" t="s">
@@ -43080,6 +43616,9 @@
       <c r="AL147" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM147" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="26" t="s">
@@ -43193,6 +43732,9 @@
       <c r="AL148" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM148" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="26" t="s">
@@ -43306,6 +43848,9 @@
       <c r="AL149" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM149" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="26" t="s">
@@ -43419,6 +43964,9 @@
       <c r="AL150" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM150" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="26" t="s">
@@ -43532,6 +44080,9 @@
       <c r="AL151" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM151" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="26" t="s">
@@ -43643,6 +44194,9 @@
         <v>0.0</v>
       </c>
       <c r="AL152" s="25" t="n">
+        <v>1.31005266E8</v>
+      </c>
+      <c r="AM152" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -43758,6 +44312,9 @@
       <c r="AL153" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM153" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="28" t="s">
@@ -43869,6 +44426,9 @@
         <v>2.10680367E8</v>
       </c>
       <c r="AL154" s="25" t="n">
+        <v>2.503109684E9</v>
+      </c>
+      <c r="AM154" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -43982,6 +44542,9 @@
         <v>2.10680367E8</v>
       </c>
       <c r="AL155" s="25" t="n">
+        <v>2.492270425E9</v>
+      </c>
+      <c r="AM155" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -44095,6 +44658,9 @@
         <v>0.0</v>
       </c>
       <c r="AL156" s="25" t="n">
+        <v>1.0839259E7</v>
+      </c>
+      <c r="AM156" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -44210,6 +44776,9 @@
       <c r="AL157" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM157" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="26" t="s">
@@ -44323,6 +44892,9 @@
       <c r="AL158" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM158" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="26" t="s">
@@ -44436,6 +45008,9 @@
       <c r="AL159" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM159" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="26" t="s">
@@ -44549,6 +45124,9 @@
       <c r="AL160" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM160" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="26" t="s">
@@ -44662,6 +45240,9 @@
       <c r="AL161" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM161" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="26" t="s">
@@ -44775,6 +45356,9 @@
       <c r="AL162" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM162" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="28" t="s">
@@ -44888,6 +45472,9 @@
       <c r="AL163" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM163" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="26" t="s">
@@ -45001,6 +45588,9 @@
       <c r="AL164" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM164" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="26" t="s">
@@ -45114,6 +45704,9 @@
       <c r="AL165" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM165" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="26" t="s">
@@ -45227,6 +45820,9 @@
       <c r="AL166" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM166" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="26" t="s">
@@ -45340,6 +45936,9 @@
       <c r="AL167" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM167" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="26" t="s">
@@ -45451,6 +46050,9 @@
         <v>0.0</v>
       </c>
       <c r="AL168" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AM168" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -45492,7 +46094,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="J10:AL10"/>
+    <mergeCell ref="J10:AM10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A174" r:id="rId1" display="https://www.vietcap.com.vn/" xr:uid="{D6386FB0-752A-884E-829A-45A876D98EB2}"/>

</xml_diff>